<commit_message>
Add UN population data
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whotilities/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A67BB28-BD83-3142-A406-6E3816F08AEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E040E9-65C7-2C40-910B-56BAF8BE39C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="227">
   <si>
     <t>AFG</t>
   </si>
@@ -633,9 +633,6 @@
     <t>Czech Republic</t>
   </si>
   <si>
-    <t>United Kingdom of Great Britain and Northern Ireland</t>
-  </si>
-  <si>
     <t>Bolivarian Republic of Venezuela</t>
   </si>
   <si>
@@ -703,6 +700,21 @@
   </si>
   <si>
     <t>Venezuela</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>ESH</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Micronesia (Fed. States of)</t>
+  </si>
+  <si>
+    <t>Dem. People's Republic of Korea</t>
   </si>
 </sst>
 </file>
@@ -1084,11 +1096,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D195"/>
+  <dimension ref="A1:D196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C192" sqref="C192"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1101,13 +1113,13 @@
         <v>195</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1170,7 +1182,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1218,7 +1230,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1241,7 +1253,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1264,7 +1276,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1317,7 +1329,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1335,7 +1347,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1366,7 +1378,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="C48" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1374,7 +1389,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1540,7 +1555,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1608,7 +1623,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -1621,17 +1636,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -1639,72 +1654,75 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="C112" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
@@ -1847,7 +1865,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
@@ -1855,7 +1873,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
@@ -1988,7 +2006,7 @@
         <v>165</v>
       </c>
       <c r="D167" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -2029,7 +2047,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -2087,10 +2105,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="C185" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
@@ -2098,7 +2116,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
@@ -2129,10 +2147,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C191" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
@@ -2140,22 +2158,30 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>223</v>
+      </c>
+      <c r="B196" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2383,18 +2409,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2417,6 +2443,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D36B4478-A2EE-4785-989A-82A85AB662CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2431,12 +2465,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to version 0.1.2
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whotilities/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E040E9-65C7-2C40-910B-56BAF8BE39C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5358458-D0D8-354F-BE95-E1DF1E4DB0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
   <si>
     <t>AFG</t>
   </si>
@@ -715,6 +715,18 @@
   </si>
   <si>
     <t>Dem. People's Republic of Korea</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>TWN</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
   </si>
 </sst>
 </file>
@@ -1096,11 +1108,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D196"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2184,6 +2196,22 @@
         <v>224</v>
       </c>
     </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>227</v>
+      </c>
+      <c r="B197" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>229</v>
+      </c>
+      <c r="B198" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A195" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2192,6 +2220,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2408,15 +2445,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2424,6 +2452,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{957C67AA-7650-4602-BE08-A264C8CC3D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2438,14 +2474,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add former name for North Macedonia
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whotilities/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5358458-D0D8-354F-BE95-E1DF1E4DB0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989D7771-48F7-2343-8C52-195C363630A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="233">
   <si>
     <t>AFG</t>
   </si>
@@ -727,6 +727,12 @@
   </si>
   <si>
     <t>Taiwan</t>
+  </si>
+  <si>
+    <t>TFYR Macedonia</t>
+  </si>
+  <si>
+    <t>formername2</t>
   </si>
 </sst>
 </file>
@@ -1108,11 +1114,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D198"/>
+  <dimension ref="A1:E198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B198" sqref="B198"/>
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O182" sqref="O182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1126,7 @@
     <col min="2" max="3" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>195</v>
       </c>
@@ -1133,63 +1139,66 @@
       <c r="D1" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1197,17 +1206,17 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1983,37 +1992,37 @@
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>165</v>
       </c>
@@ -2021,40 +2030,43 @@
         <v>216</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>171</v>
       </c>
       <c r="D173" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E173" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -2062,12 +2074,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -2220,15 +2232,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2445,6 +2448,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2452,14 +2464,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{957C67AA-7650-4602-BE08-A264C8CC3D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2474,6 +2478,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add alt country names for Republic of Korea and DRC
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989D7771-48F7-2343-8C52-195C363630A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362E8213-14FB-624E-992A-FD8EADA88041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="235">
   <si>
     <t>AFG</t>
   </si>
@@ -733,6 +733,12 @@
   </si>
   <si>
     <t>formername2</t>
+  </si>
+  <si>
+    <t>Dem. Rep. of the Congo</t>
+  </si>
+  <si>
+    <t>Korea, Republic of</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1123,8 @@
   <dimension ref="A1:E198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O182" sqref="O182"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1405,85 +1411,88 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1826,70 +1835,73 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
       <c r="B140" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C140" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -1897,17 +1909,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -2232,6 +2244,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2448,15 +2469,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2464,6 +2476,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{957C67AA-7650-4602-BE08-A264C8CC3D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2478,14 +2498,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add another alt names for DRC and CAR
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362E8213-14FB-624E-992A-FD8EADA88041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93ECE6B3-B847-AB47-B743-C7658D5BBCD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="238">
   <si>
     <t>AFG</t>
   </si>
@@ -739,6 +739,15 @@
   </si>
   <si>
     <t>Korea, Republic of</t>
+  </si>
+  <si>
+    <t>altname3</t>
+  </si>
+  <si>
+    <t>DRC</t>
+  </si>
+  <si>
+    <t>CAR</t>
   </si>
 </sst>
 </file>
@@ -1120,19 +1129,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E198"/>
+  <dimension ref="A1:F198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C141" sqref="C141"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="25.5" customWidth="1"/>
+    <col min="2" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>195</v>
       </c>
@@ -1143,68 +1152,71 @@
         <v>220</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1212,17 +1224,17 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1316,42 +1328,45 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1359,17 +1374,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1377,30 +1392,30 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1411,7 +1426,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1421,161 +1436,164 @@
       <c r="C49" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2004,81 +2022,81 @@
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-      <c r="D167" t="s">
+      <c r="E167" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>171</v>
       </c>
-      <c r="D173" t="s">
+      <c r="E173" t="s">
         <v>172</v>
       </c>
-      <c r="E173" t="s">
+      <c r="F173" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -2086,12 +2104,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -2244,12 +2262,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2470,15 +2485,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D36B4478-A2EE-4785-989A-82A85AB662CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2503,18 +2530,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D36B4478-A2EE-4785-989A-82A85AB662CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update data and README
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93ECE6B3-B847-AB47-B743-C7658D5BBCD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0EE7E7-4B2B-7241-8B61-276E72FBD7D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="241">
   <si>
     <t>AFG</t>
   </si>
@@ -748,6 +748,15 @@
   </si>
   <si>
     <t>CAR</t>
+  </si>
+  <si>
+    <t>altname4</t>
+  </si>
+  <si>
+    <t>Zaire</t>
+  </si>
+  <si>
+    <t>Congo Democratic Republic</t>
   </si>
 </sst>
 </file>
@@ -1129,19 +1138,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F198"/>
+  <dimension ref="A1:G198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="25.5" customWidth="1"/>
+    <col min="2" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>195</v>
       </c>
@@ -1155,68 +1164,71 @@
         <v>235</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1224,17 +1236,17 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1328,12 +1340,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1341,32 +1353,32 @@
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1374,17 +1386,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1392,30 +1404,30 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1439,161 +1451,167 @@
       <c r="D49" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>240</v>
+      </c>
+      <c r="F49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2022,81 +2040,81 @@
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-      <c r="E167" t="s">
+      <c r="F167" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>171</v>
       </c>
-      <c r="E173" t="s">
+      <c r="F173" t="s">
         <v>172</v>
       </c>
-      <c r="F173" t="s">
+      <c r="G173" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -2104,12 +2122,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -2262,12 +2280,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2484,16 +2511,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D36B4478-A2EE-4785-989A-82A85AB662CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2510,7 +2536,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{957C67AA-7650-4602-BE08-A264C8CC3D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2527,12 +2553,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add "Macedonia (TFYR)" to altnames
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0EE7E7-4B2B-7241-8B61-276E72FBD7D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFA6233-1CD5-E64C-BB1C-B825941CE76D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="region" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="242">
   <si>
     <t>AFG</t>
   </si>
@@ -757,6 +757,9 @@
   </si>
   <si>
     <t>Congo Democratic Republic</t>
+  </si>
+  <si>
+    <t>Macedonia (TFYR)</t>
   </si>
 </sst>
 </file>
@@ -1141,8 +1144,8 @@
   <dimension ref="A1:G198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2107,6 +2110,9 @@
       <c r="A173" t="s">
         <v>171</v>
       </c>
+      <c r="B173" t="s">
+        <v>241</v>
+      </c>
       <c r="F173" t="s">
         <v>172</v>
       </c>
@@ -2280,18 +2286,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2512,14 +2518,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D36B4478-A2EE-4785-989A-82A85AB662CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2532,6 +2530,14 @@
     <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Close #1, update to 0.1.4
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFA6233-1CD5-E64C-BB1C-B825941CE76D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC2B189-7BA0-4248-897A-2AF327657DDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="252">
   <si>
     <t>AFG</t>
   </si>
@@ -760,6 +760,36 @@
   </si>
   <si>
     <t>Macedonia (TFYR)</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Tanzania (United Republic of)</t>
+  </si>
+  <si>
+    <t>Palestine, State of</t>
+  </si>
+  <si>
+    <t>Moldova (Republic of)</t>
+  </si>
+  <si>
+    <t>Korea (Republic of)</t>
+  </si>
+  <si>
+    <t>HKG</t>
+  </si>
+  <si>
+    <t>Hong Kong, China (SAR)</t>
+  </si>
+  <si>
+    <t>Eswatini (Kingdom of)</t>
+  </si>
+  <si>
+    <t>altname5</t>
+  </si>
+  <si>
+    <t>Congo (Democratic Republic of the)</t>
   </si>
 </sst>
 </file>
@@ -1141,19 +1171,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G198"/>
+  <dimension ref="A1:H199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="5" width="25.5" customWidth="1"/>
+    <col min="2" max="6" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>195</v>
       </c>
@@ -1170,68 +1200,71 @@
         <v>238</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1239,17 +1272,17 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1343,12 +1376,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1356,32 +1389,32 @@
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1389,17 +1422,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1407,30 +1440,30 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1441,7 +1474,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1458,163 +1491,166 @@
         <v>240</v>
       </c>
       <c r="F49" t="s">
+        <v>251</v>
+      </c>
+      <c r="G49" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1874,62 +1910,62 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -1939,26 +1975,32 @@
       <c r="C140" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
       <c r="B141" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C141" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -2043,84 +2085,87 @@
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-      <c r="F167" t="s">
+      <c r="B167" t="s">
+        <v>249</v>
+      </c>
+      <c r="G167" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>171</v>
       </c>
       <c r="B173" t="s">
         <v>241</v>
       </c>
-      <c r="F173" t="s">
+      <c r="G173" t="s">
         <v>172</v>
       </c>
-      <c r="G173" t="s">
+      <c r="H173" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -2128,12 +2173,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -2196,6 +2241,9 @@
       <c r="B186" t="s">
         <v>210</v>
       </c>
+      <c r="C186" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
@@ -2204,6 +2252,9 @@
       <c r="B187" t="s">
         <v>186</v>
       </c>
+      <c r="C187" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
@@ -2239,22 +2290,22 @@
         <v>211</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>223</v>
       </c>
@@ -2262,20 +2313,31 @@
         <v>224</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>227</v>
       </c>
       <c r="B197" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C197" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>229</v>
       </c>
       <c r="B198" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>247</v>
+      </c>
+      <c r="B199" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2286,18 +2348,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2518,6 +2580,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D36B4478-A2EE-4785-989A-82A85AB662CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2530,14 +2600,6 @@
     <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add additional alternative names to countries df
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC2B189-7BA0-4248-897A-2AF327657DDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A42E01E-B403-9540-BA23-A05CE9172848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="255">
   <si>
     <t>AFG</t>
   </si>
@@ -790,6 +790,15 @@
   </si>
   <si>
     <t>Congo (Democratic Republic of the)</t>
+  </si>
+  <si>
+    <t>West Bank and Gaza Strip</t>
+  </si>
+  <si>
+    <t>FRO</t>
+  </si>
+  <si>
+    <t>Faeroe Islands</t>
   </si>
 </sst>
 </file>
@@ -1171,11 +1180,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H199"/>
+  <dimension ref="A1:H200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2290,22 +2299,22 @@
         <v>211</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>223</v>
       </c>
@@ -2313,7 +2322,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>227</v>
       </c>
@@ -2323,8 +2332,11 @@
       <c r="C197" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D197" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>229</v>
       </c>
@@ -2332,12 +2344,20 @@
         <v>230</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>247</v>
       </c>
       <c r="B199" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>253</v>
+      </c>
+      <c r="B200" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2357,12 +2377,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2579,6 +2593,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
   <ds:schemaRefs>
@@ -2588,23 +2608,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D36B4478-A2EE-4785-989A-82A85AB662CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
-    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{957C67AA-7650-4602-BE08-A264C8CC3D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2621,4 +2624,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D36B4478-A2EE-4785-989A-82A85AB662CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bd879b36-96f5-4c4e-979a-9eb1cd712529"/>
+    <ds:schemaRef ds:uri="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add alt name for Micronesia
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A42E01E-B403-9540-BA23-A05CE9172848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59FDAEA-CC6B-B747-90C8-983A3769306F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="256">
   <si>
     <t>AFG</t>
   </si>
@@ -799,6 +799,9 @@
   </si>
   <si>
     <t>Faeroe Islands</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
   </si>
 </sst>
 </file>
@@ -1183,8 +1186,8 @@
   <dimension ref="A1:H200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C198" sqref="C198"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1750,17 +1753,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -1768,67 +1771,67 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -1837,6 +1840,9 @@
       </c>
       <c r="C112" t="s">
         <v>225</v>
+      </c>
+      <c r="D112" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
@@ -2368,15 +2374,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2593,6 +2590,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2600,14 +2606,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{957C67AA-7650-4602-BE08-A264C8CC3D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2622,6 +2620,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Changed the name of Turkey in the raw-data spread sheets. Put the previous spelling as an altname.
</commit_message>
<xml_diff>
--- a/data-raw/alt_countries.xlsx
+++ b/data-raw/alt_countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/whoville/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vasa/who/whoville/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59FDAEA-CC6B-B747-90C8-983A3769306F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D481F027-1E6F-3944-8DD9-9A48C3C6D0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="640" windowWidth="23540" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="region" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="257">
   <si>
     <t>AFG</t>
   </si>
@@ -802,6 +802,9 @@
   </si>
   <si>
     <t>Micronesia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
   </si>
 </sst>
 </file>
@@ -1186,8 +1189,8 @@
   <dimension ref="A1:H200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2212,6 +2215,9 @@
       <c r="A179" t="s">
         <v>178</v>
       </c>
+      <c r="B179" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
@@ -2374,6 +2380,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -2590,15 +2605,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2606,6 +2612,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{957C67AA-7650-4602-BE08-A264C8CC3D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2620,14 +2634,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF7CB392-C6BC-4EAB-B766-186EA72B989D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>